<commit_message>
Modification des Headings et du titre de la page
</commit_message>
<xml_diff>
--- a/audit-SEO-25_07_2021.xlsx
+++ b/audit-SEO-25_07_2021.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="945" yWindow="615" windowWidth="27855" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="audit" sheetId="1" r:id="rId1"/>
+    <sheet name="captures-ecrans" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>Catégorie</t>
   </si>
@@ -144,13 +145,37 @@
     <t>Un élément de la page n'est pas définit</t>
   </si>
   <si>
-    <t>L'élément  Toggle navigation apparait au millue de la page</t>
-  </si>
-  <si>
-    <t>La apge doit avoir tout ses éleements identifiables</t>
-  </si>
-  <si>
     <t>supprimer lélément</t>
+  </si>
+  <si>
+    <t>Le titre se termine par un point</t>
+  </si>
+  <si>
+    <t>La page doit avoir tout ses éléments identifiables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les éléments doivent être hierachisés H1 et h2 et h3 </t>
+  </si>
+  <si>
+    <t>Hiérachisé les balise headings</t>
+  </si>
+  <si>
+    <t>Eléments heading non correctes</t>
+  </si>
+  <si>
+    <t>La hierachisation des élément H1/h2/h3 n'est pas correctés sur les pages</t>
+  </si>
+  <si>
+    <t>Le titre c'est la marque de l'agence et la marque n'a pas de point</t>
+  </si>
+  <si>
+    <t>Ne pas ajouter de ponctuation à une marque</t>
+  </si>
+  <si>
+    <t>Retirer le point</t>
+  </si>
+  <si>
+    <t>L'élément  Toggle navigation apparait au millieu de la page</t>
   </si>
 </sst>
 </file>
@@ -190,7 +215,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +226,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -223,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +273,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,6 +289,293 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="990600" y="190500"/>
+          <a:ext cx="3190875" cy="2990850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>187005</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1362076" y="3733800"/>
+          <a:ext cx="3158804" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>246185</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2051" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7305675" y="3657600"/>
+          <a:ext cx="3217985" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7305675" y="190500"/>
+          <a:ext cx="3257550" cy="2981325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2053" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1362075" y="6667500"/>
+          <a:ext cx="3200400" cy="4086225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2054" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7315200" y="6638925"/>
+          <a:ext cx="2867025" cy="3886200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,15 +779,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="52.5546875" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" customWidth="1"/>
+    <col min="4" max="4" width="42.88671875" customWidth="1"/>
     <col min="5" max="5" width="33.44140625" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
@@ -659,19 +981,19 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -734,31 +1056,63 @@
         <v>38</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="7" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>41</v>
+      <c r="C18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1731,4 +2085,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>